<commit_message>
Edited Tesseract OCR Model files for use in video presentation.
</commit_message>
<xml_diff>
--- a/backend/model/tesseract_evaluation_results.xlsx
+++ b/backend/model/tesseract_evaluation_results.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wenji\Desktop\NUS Academics\NUS Y3S1\DSA3101\dsa3101-2310-12-ocr\backend\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFDD4F68-A01D-4BC9-84A2-757C3B3D63A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D99418-E116-4A49-9D31-9F4A08AFAC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2261,12 +2260,12 @@
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+      <selection activeCell="F1" sqref="F1:F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>